<commit_message>
🔐 Updated passwords in logistics_system_sheets.xlsx
</commit_message>
<xml_diff>
--- a/logistics_system_sheets.xlsx
+++ b/logistics_system_sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEB99A0-CB7C-4E92-9200-2EB3FFDED791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE56A48A-DFCE-42B3-B1E0-BD16D8FD06B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="408">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1706" uniqueCount="409">
   <si>
     <t>username</t>
   </si>
@@ -1246,6 +1246,9 @@
   </si>
   <si>
     <t>P04420</t>
+  </si>
+  <si>
+    <t>A123</t>
   </si>
 </sst>
 </file>
@@ -1636,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F224"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="E223" sqref="E223"/>
+    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
+      <selection activeCell="D222" sqref="D222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5980,8 +5983,8 @@
       <c r="A222" t="s">
         <v>243</v>
       </c>
-      <c r="B222">
-        <v>1234</v>
+      <c r="B222" t="s">
+        <v>408</v>
       </c>
       <c r="C222" t="s">
         <v>244</v>
@@ -5997,8 +6000,8 @@
       <c r="A223" t="s">
         <v>247</v>
       </c>
-      <c r="B223">
-        <v>1234</v>
+      <c r="B223" t="s">
+        <v>247</v>
       </c>
       <c r="C223" t="s">
         <v>248</v>
@@ -6039,7 +6042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
🔥 Fix: Removed merge conflict leftovers
</commit_message>
<xml_diff>
--- a/logistics_system_sheets.xlsx
+++ b/logistics_system_sheets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE56A48A-DFCE-42B3-B1E0-BD16D8FD06B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33E8F14B-BB21-4A82-AE5F-52A251B62667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1639,8 +1639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="D222" sqref="D222"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2677,7 +2677,7 @@
         <v>60</v>
       </c>
       <c r="C52" t="s">
-        <v>61</v>
+        <v>259</v>
       </c>
       <c r="D52" t="s">
         <v>8</v>
@@ -2711,7 +2711,7 @@
         <v>67</v>
       </c>
       <c r="C54" t="s">
-        <v>61</v>
+        <v>259</v>
       </c>
       <c r="D54" t="s">
         <v>8</v>
@@ -2745,7 +2745,7 @@
         <v>71</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>259</v>
       </c>
       <c r="D56" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fix: dynamic columns when adding new transfer to match Excel sheet
</commit_message>
<xml_diff>
--- a/logistics_system_sheets.xlsx
+++ b/logistics_system_sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E90856-323C-4CBD-A375-B8D8195282B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32863CA9-3984-4C50-ADB2-777477B4500C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -804,18 +804,6 @@
     <t>driver</t>
   </si>
   <si>
-    <t>Transfer Type</t>
-  </si>
-  <si>
-    <t>Handled By WH</t>
-  </si>
-  <si>
-    <t>Attachment</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Branch Code</t>
   </si>
   <si>
@@ -1249,6 +1237,18 @@
   </si>
   <si>
     <t>received_at</t>
+  </si>
+  <si>
+    <t>attachment</t>
+  </si>
+  <si>
+    <t>handled_by_wh</t>
+  </si>
+  <si>
+    <t>transfer_type</t>
+  </si>
+  <si>
+    <t>Notes.</t>
   </si>
 </sst>
 </file>
@@ -5984,7 +5984,7 @@
         <v>243</v>
       </c>
       <c r="B222" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C222" t="s">
         <v>244</v>
@@ -6043,12 +6043,15 @@
   <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="10" max="10" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -6077,22 +6080,22 @@
         <v>259</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>260</v>
+        <v>407</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>408</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>
@@ -6110,10 +6113,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -6518,7 +6521,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B52" t="s">
         <v>76</v>
@@ -6526,7 +6529,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B53" t="s">
         <v>76</v>
@@ -6534,7 +6537,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B54" t="s">
         <v>76</v>
@@ -6542,7 +6545,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B55" t="s">
         <v>76</v>
@@ -6550,7 +6553,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B56" t="s">
         <v>76</v>
@@ -6558,7 +6561,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B57" t="s">
         <v>76</v>
@@ -6566,7 +6569,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B58" t="s">
         <v>76</v>
@@ -6574,7 +6577,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B59" t="s">
         <v>76</v>
@@ -6582,7 +6585,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B60" t="s">
         <v>76</v>
@@ -6590,7 +6593,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B61" t="s">
         <v>76</v>
@@ -6598,7 +6601,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B62" t="s">
         <v>76</v>
@@ -6606,7 +6609,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B63" t="s">
         <v>76</v>
@@ -6614,7 +6617,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B64" t="s">
         <v>76</v>
@@ -6622,7 +6625,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="B65" t="s">
         <v>76</v>
@@ -6630,7 +6633,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B66" t="s">
         <v>76</v>
@@ -6638,7 +6641,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B67" t="s">
         <v>76</v>
@@ -6646,7 +6649,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B68" t="s">
         <v>76</v>
@@ -6654,7 +6657,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B69" t="s">
         <v>76</v>
@@ -6662,7 +6665,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B70" t="s">
         <v>76</v>
@@ -6670,7 +6673,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B71" t="s">
         <v>76</v>
@@ -6678,7 +6681,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B72" t="s">
         <v>76</v>
@@ -6686,7 +6689,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B73" t="s">
         <v>76</v>
@@ -6694,7 +6697,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B74" t="s">
         <v>76</v>
@@ -6702,7 +6705,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B75" t="s">
         <v>76</v>
@@ -6710,7 +6713,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B76" t="s">
         <v>76</v>
@@ -6718,7 +6721,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B77" t="s">
         <v>76</v>
@@ -6726,7 +6729,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B78" t="s">
         <v>76</v>
@@ -6734,7 +6737,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B79" t="s">
         <v>76</v>
@@ -6742,7 +6745,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B80" t="s">
         <v>76</v>
@@ -6750,7 +6753,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="B81" t="s">
         <v>76</v>
@@ -6758,7 +6761,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B82" t="s">
         <v>76</v>
@@ -6766,7 +6769,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B83" t="s">
         <v>76</v>
@@ -6774,7 +6777,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B84" t="s">
         <v>76</v>
@@ -6782,7 +6785,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B85" t="s">
         <v>76</v>
@@ -6790,7 +6793,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B86" t="s">
         <v>76</v>
@@ -6798,7 +6801,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B87" t="s">
         <v>76</v>
@@ -6806,7 +6809,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B88" t="s">
         <v>76</v>
@@ -6814,7 +6817,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B89" t="s">
         <v>76</v>
@@ -6822,7 +6825,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B90" t="s">
         <v>76</v>
@@ -6830,7 +6833,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B91" t="s">
         <v>76</v>
@@ -6838,7 +6841,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B92" t="s">
         <v>76</v>
@@ -6846,7 +6849,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B93" t="s">
         <v>76</v>
@@ -6854,7 +6857,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B94" t="s">
         <v>76</v>
@@ -6862,7 +6865,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B95" t="s">
         <v>76</v>
@@ -6870,7 +6873,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B96" t="s">
         <v>76</v>
@@ -6878,7 +6881,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="B97" t="s">
         <v>76</v>
@@ -6886,7 +6889,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B98" t="s">
         <v>76</v>
@@ -6894,7 +6897,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B99" t="s">
         <v>76</v>
@@ -6902,7 +6905,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B100" t="s">
         <v>76</v>
@@ -6910,7 +6913,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="B101" t="s">
         <v>76</v>
@@ -6918,7 +6921,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B102" t="s">
         <v>133</v>
@@ -6926,7 +6929,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="B103" t="s">
         <v>133</v>
@@ -6934,7 +6937,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B104" t="s">
         <v>133</v>
@@ -6942,7 +6945,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B105" t="s">
         <v>133</v>
@@ -6950,7 +6953,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B106" t="s">
         <v>133</v>
@@ -6958,7 +6961,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B107" t="s">
         <v>133</v>
@@ -6966,7 +6969,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B108" t="s">
         <v>133</v>
@@ -6974,7 +6977,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="B109" t="s">
         <v>133</v>
@@ -6982,7 +6985,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="B110" t="s">
         <v>133</v>
@@ -6990,7 +6993,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B111" t="s">
         <v>133</v>
@@ -6998,7 +7001,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B112" t="s">
         <v>133</v>
@@ -7006,7 +7009,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B113" t="s">
         <v>133</v>
@@ -7014,7 +7017,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B114" t="s">
         <v>133</v>
@@ -7022,7 +7025,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B115" t="s">
         <v>133</v>
@@ -7030,7 +7033,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B116" t="s">
         <v>133</v>
@@ -7038,7 +7041,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B117" t="s">
         <v>133</v>
@@ -7046,7 +7049,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B118" t="s">
         <v>133</v>
@@ -7054,7 +7057,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B119" t="s">
         <v>133</v>
@@ -7062,7 +7065,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B120" t="s">
         <v>133</v>
@@ -7070,7 +7073,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="B121" t="s">
         <v>133</v>
@@ -7078,7 +7081,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B122" t="s">
         <v>133</v>
@@ -7086,7 +7089,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B123" t="s">
         <v>133</v>
@@ -7094,7 +7097,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B124" t="s">
         <v>133</v>
@@ -7102,7 +7105,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="B125" t="s">
         <v>133</v>
@@ -7110,7 +7113,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B126" t="s">
         <v>133</v>
@@ -7118,7 +7121,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="B127" t="s">
         <v>133</v>
@@ -7126,7 +7129,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="B128" t="s">
         <v>133</v>
@@ -7134,7 +7137,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="B129" t="s">
         <v>133</v>
@@ -7142,7 +7145,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="B130" t="s">
         <v>133</v>
@@ -7150,7 +7153,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B131" t="s">
         <v>133</v>
@@ -7158,7 +7161,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B132" t="s">
         <v>133</v>
@@ -7166,7 +7169,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="B133" t="s">
         <v>133</v>
@@ -7174,7 +7177,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B134" t="s">
         <v>133</v>
@@ -7182,7 +7185,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="B135" t="s">
         <v>133</v>
@@ -7190,7 +7193,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="B136" t="s">
         <v>133</v>
@@ -7198,7 +7201,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B137" t="s">
         <v>133</v>
@@ -7206,7 +7209,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="B138" t="s">
         <v>133</v>
@@ -7214,7 +7217,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="B139" t="s">
         <v>133</v>
@@ -7222,7 +7225,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B140" t="s">
         <v>133</v>
@@ -7230,7 +7233,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B141" t="s">
         <v>133</v>
@@ -7238,7 +7241,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B142" t="s">
         <v>133</v>
@@ -7246,7 +7249,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B143" t="s">
         <v>133</v>
@@ -7254,7 +7257,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B144" t="s">
         <v>133</v>
@@ -7262,7 +7265,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B145" t="s">
         <v>133</v>
@@ -7270,7 +7273,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="B146" t="s">
         <v>133</v>
@@ -7278,7 +7281,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="B147" t="s">
         <v>133</v>
@@ -7286,7 +7289,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="B148" t="s">
         <v>133</v>
@@ -7294,7 +7297,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="B149" t="s">
         <v>133</v>
@@ -7302,7 +7305,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B150" t="s">
         <v>133</v>
@@ -7310,7 +7313,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="B151" t="s">
         <v>133</v>
@@ -7318,7 +7321,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="B152" t="s">
         <v>190</v>
@@ -7326,7 +7329,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B153" t="s">
         <v>190</v>
@@ -7334,7 +7337,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B154" t="s">
         <v>190</v>
@@ -7342,7 +7345,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B155" t="s">
         <v>190</v>
@@ -7350,7 +7353,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B156" t="s">
         <v>190</v>
@@ -7358,7 +7361,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="B157" t="s">
         <v>190</v>
@@ -7366,7 +7369,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="B158" t="s">
         <v>190</v>
@@ -7374,7 +7377,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B159" t="s">
         <v>190</v>
@@ -7382,7 +7385,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="B160" t="s">
         <v>190</v>
@@ -7390,7 +7393,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B161" t="s">
         <v>190</v>
@@ -7398,7 +7401,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B162" t="s">
         <v>190</v>
@@ -7406,7 +7409,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B163" t="s">
         <v>190</v>
@@ -7414,7 +7417,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B164" t="s">
         <v>190</v>
@@ -7422,7 +7425,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B165" t="s">
         <v>190</v>
@@ -7430,7 +7433,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B166" t="s">
         <v>190</v>
@@ -7438,7 +7441,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B167" t="s">
         <v>190</v>
@@ -7446,7 +7449,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B168" t="s">
         <v>190</v>
@@ -7454,7 +7457,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B169" t="s">
         <v>190</v>
@@ -7462,7 +7465,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="B170" t="s">
         <v>190</v>
@@ -7470,7 +7473,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="B171" t="s">
         <v>190</v>
@@ -7478,7 +7481,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B172" t="s">
         <v>217</v>
@@ -7486,7 +7489,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B173" t="s">
         <v>217</v>
@@ -7494,7 +7497,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="B174" t="s">
         <v>217</v>
@@ -7502,7 +7505,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="B175" t="s">
         <v>217</v>
@@ -7510,7 +7513,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B176" t="s">
         <v>217</v>
@@ -7518,7 +7521,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B177" t="s">
         <v>217</v>
@@ -7526,7 +7529,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="B178" t="s">
         <v>217</v>
@@ -7534,7 +7537,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B179" t="s">
         <v>217</v>
@@ -7542,7 +7545,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="B180" t="s">
         <v>217</v>
@@ -7550,7 +7553,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="B181" t="s">
         <v>217</v>
@@ -7558,7 +7561,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B182" t="s">
         <v>217</v>
@@ -7566,7 +7569,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B183" t="s">
         <v>217</v>
@@ -7574,7 +7577,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="B184" t="s">
         <v>217</v>
@@ -7582,7 +7585,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="B185" t="s">
         <v>217</v>
@@ -7590,7 +7593,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="B186" t="s">
         <v>217</v>
@@ -7598,7 +7601,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="B187" t="s">
         <v>217</v>
@@ -7606,7 +7609,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="B188" t="s">
         <v>217</v>
@@ -7614,7 +7617,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="B189" t="s">
         <v>217</v>
@@ -7622,7 +7625,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="B190" t="s">
         <v>217</v>
@@ -7630,7 +7633,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="B191" t="s">
         <v>217</v>

</xml_diff>

<commit_message>
Fix: bug where transfer was not saved, change ExcelWriter mode to w
</commit_message>
<xml_diff>
--- a/logistics_system_sheets.xlsx
+++ b/logistics_system_sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D27941-7346-49F4-900E-EB14A140B0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14D1EC5F-E116-4F13-BF84-CD3C5091689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2832" yWindow="1968" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>

</xml_diff>